<commit_message>
added excel data loader
</commit_message>
<xml_diff>
--- a/Sample/input/Test_Data.xlsx
+++ b/Sample/input/Test_Data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Browser</t>
   </si>
@@ -23,19 +23,40 @@
     <t>Search</t>
   </si>
   <si>
-    <t>http://www.google.com</t>
-  </si>
-  <si>
-    <t>Apple</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
+    <t>TC1</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>TC2</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>TC3</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>TC4</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>D1</t>
   </si>
 </sst>
 </file>
@@ -45,7 +66,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -67,13 +88,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF2A00FF"/>
-      <name val="Monaco"/>
-      <family val="3"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -118,16 +132,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -140,66 +150,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF2A00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -208,53 +158,70 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="14.4285714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="http://www.google.com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Added remote execution handler
</commit_message>
<xml_diff>
--- a/Sample/input/Test_Data.xlsx
+++ b/Sample/input/Test_Data.xlsx
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
-  <si>
-    <t xml:space="preserve">Browser</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t xml:space="preserve">Search</t>
   </si>
@@ -32,9 +29,6 @@
   </si>
   <si>
     <t xml:space="preserve">TC1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chrome</t>
   </si>
   <si>
     <t xml:space="preserve">Apple</t>
@@ -134,10 +128,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -152,22 +146,16 @@
       <c r="C1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>4</v>
-      </c>
       <c r="C2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>